<commit_message>
Completed ResultsTests.  Changed app to use club name instead of id.
</commit_message>
<xml_diff>
--- a/data/poission.xlsx
+++ b/data/poission.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="20940" windowHeight="10110"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20940" windowHeight="10110" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Figueroa" sheetId="7" r:id="rId1"/>
     <sheet name="AlHabsi" sheetId="6" r:id="rId2"/>
     <sheet name="Four games" sheetId="4" r:id="rId3"/>
     <sheet name="Three games" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Average Goals Calc" sheetId="2" r:id="rId5"/>
+    <sheet name="Six Games" sheetId="3" r:id="rId6"/>
     <sheet name="Mignolet Points" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="181">
   <si>
     <t>Wigan</t>
   </si>
@@ -356,6 +357,213 @@
   </si>
   <si>
     <t>bonus</t>
+  </si>
+  <si>
+    <t>home goals</t>
+  </si>
+  <si>
+    <t>away goals</t>
+  </si>
+  <si>
+    <t>number of results</t>
+  </si>
+  <si>
+    <t>away goals baseline</t>
+  </si>
+  <si>
+    <t>home goals baseline</t>
+  </si>
+  <si>
+    <t>average goals</t>
+  </si>
+  <si>
+    <t>attack strength</t>
+  </si>
+  <si>
+    <t>average teamB conceded</t>
+  </si>
+  <si>
+    <t>average teamA scored</t>
+  </si>
+  <si>
+    <t>defence weakness</t>
+  </si>
+  <si>
+    <t>expected home goals</t>
+  </si>
+  <si>
+    <t>expected away goals</t>
+  </si>
+  <si>
+    <t>home team scored</t>
+  </si>
+  <si>
+    <t>home team conceded</t>
+  </si>
+  <si>
+    <t>home team games</t>
+  </si>
+  <si>
+    <t>away team scored</t>
+  </si>
+  <si>
+    <t>home conceded</t>
+  </si>
+  <si>
+    <t>average home team conceded</t>
+  </si>
+  <si>
+    <t>away conceded</t>
+  </si>
+  <si>
+    <t>away games</t>
+  </si>
+  <si>
+    <t>home defence weakness</t>
+  </si>
+  <si>
+    <t>average away team scored</t>
+  </si>
+  <si>
+    <t>average away team conceded</t>
+  </si>
+  <si>
+    <t>away defence weakness</t>
+  </si>
+  <si>
+    <t>average home team goals</t>
+  </si>
+  <si>
+    <t>home team attack strength</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>For</t>
+  </si>
+  <si>
+    <t>Against</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Defence</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Blackburn</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Aston Villa</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Bolton</t>
+  </si>
+  <si>
+    <t>West Brom</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Sunderland</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
+  </si>
+  <si>
+    <t>Man City</t>
+  </si>
+  <si>
+    <t>Man United</t>
+  </si>
+  <si>
+    <t>Swansea</t>
+  </si>
+  <si>
+    <t>QPR</t>
+  </si>
+  <si>
+    <t>Stoke</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Norwich</t>
+  </si>
+  <si>
+    <t>Average Home Goals</t>
+  </si>
+  <si>
+    <t>Average Away Goals</t>
+  </si>
+  <si>
+    <t>everton newcastle</t>
+  </si>
+  <si>
+    <t>home scored</t>
+  </si>
+  <si>
+    <t>home played</t>
+  </si>
+  <si>
+    <t>away scored</t>
+  </si>
+  <si>
+    <t>away played</t>
+  </si>
+  <si>
+    <t>Total Home Goals</t>
+  </si>
+  <si>
+    <t>Total Away Goals</t>
+  </si>
+  <si>
+    <t>Games Played</t>
+  </si>
+  <si>
+    <t>played</t>
+  </si>
+  <si>
+    <t>west brom arsenal</t>
+  </si>
+  <si>
+    <t>stoke bolton</t>
+  </si>
+  <si>
+    <t>norwich aston villa</t>
+  </si>
+  <si>
+    <t>chelsea blackburn</t>
+  </si>
+  <si>
+    <t>swansea liverpool</t>
+  </si>
+  <si>
+    <t>man city qpr</t>
+  </si>
+  <si>
+    <t>tottenham fulham</t>
+  </si>
+  <si>
+    <t>sunderland man united</t>
   </si>
 </sst>
 </file>
@@ -412,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
@@ -422,6 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -724,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S40" workbookViewId="0">
-      <selection activeCell="AC59" sqref="AC59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1702,14 +1911,14 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
       <c r="M16" s="2">
         <v>41611.833333333336</v>
       </c>
@@ -1855,11 +2064,11 @@
         <v>0.9861534547738493</v>
       </c>
       <c r="C18">
-        <f>POISSON(C17,$B$13,FALSE)</f>
+        <f t="shared" ref="C18:H18" si="0">POISSON(C17,$B$13,FALSE)</f>
         <v>0.14660696213035052</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:H18" si="0">POISSON(D17,$B$13,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.28148536729027301</v>
       </c>
       <c r="E18">
@@ -1937,14 +2146,14 @@
       </c>
     </row>
     <row r="19" spans="1:31">
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
       <c r="M19" s="2">
         <v>41630.53125</v>
       </c>
@@ -2242,16 +2451,16 @@
       </c>
     </row>
     <row r="23" spans="1:31">
-      <c r="C23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="M23" s="2">
         <v>41286.625</v>
       </c>
@@ -2394,7 +2603,7 @@
       </c>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B25">
@@ -2495,7 +2704,7 @@
       </c>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -2594,7 +2803,7 @@
       </c>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>2</v>
       </c>
@@ -2693,7 +2902,7 @@
       </c>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>3</v>
       </c>
@@ -2792,7 +3001,7 @@
       </c>
     </row>
     <row r="29" spans="1:31">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>4</v>
       </c>
@@ -2891,7 +3100,7 @@
       </c>
     </row>
     <row r="30" spans="1:31">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30">
         <v>5</v>
       </c>
@@ -3409,7 +3618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="17:29">
+    <row r="49" spans="17:30">
       <c r="Q49">
         <v>0</v>
       </c>
@@ -3432,7 +3641,7 @@
         <v>1.3588379880148507E-2</v>
       </c>
       <c r="X49">
-        <f>S49*(S$48*0.2)</f>
+        <f t="shared" ref="X49:X54" si="7">S49*(S$48*0.2)</f>
         <v>4.7403343002356008E-3</v>
       </c>
       <c r="Y49">
@@ -3452,7 +3661,7 @@
         <v>1.3588379880148507E-2</v>
       </c>
     </row>
-    <row r="50" spans="17:29">
+    <row r="50" spans="17:30">
       <c r="Q50">
         <v>1</v>
       </c>
@@ -3475,27 +3684,27 @@
         <v>2.6089689369885136E-2</v>
       </c>
       <c r="X50">
-        <f>S50*(S$48*0.2)</f>
+        <f t="shared" si="7"/>
         <v>9.1014418564523535E-3</v>
       </c>
       <c r="Y50">
-        <f>T50*(T$48*0.2)</f>
+        <f t="shared" ref="Y50:AB54" si="8">T50*(T$48*0.2)</f>
         <v>2.6212152546582781E-2</v>
       </c>
       <c r="Z50">
-        <f>U50*(U$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>3.7745499667079199E-2</v>
       </c>
       <c r="AA50">
-        <f>V50*(V$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>3.6235679680396031E-2</v>
       </c>
       <c r="AB50">
-        <f>W50*(W$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.6089689369885136E-2</v>
       </c>
     </row>
-    <row r="51" spans="17:29">
+    <row r="51" spans="17:30">
       <c r="Q51">
         <v>2</v>
       </c>
@@ -3518,27 +3727,27 @@
         <v>2.5046101795089735E-2</v>
       </c>
       <c r="X51">
-        <f>S51*(S$48*0.2)</f>
+        <f t="shared" si="7"/>
         <v>8.7373841821942622E-3</v>
       </c>
       <c r="Y51">
-        <f>T51*(T$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.5163666444719474E-2</v>
       </c>
       <c r="Z51">
-        <f>U51*(U$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>3.6235679680396045E-2</v>
       </c>
       <c r="AA51">
-        <f>V51*(V$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>3.4786252493180202E-2</v>
       </c>
       <c r="AB51">
-        <f>W51*(W$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.5046101795089735E-2</v>
       </c>
     </row>
-    <row r="52" spans="17:29">
+    <row r="52" spans="17:30">
       <c r="Q52">
         <v>3</v>
       </c>
@@ -3561,27 +3770,27 @@
         <v>1.6029505148857433E-2</v>
       </c>
       <c r="X52">
-        <f>S52*(S$48*0.2)</f>
+        <f t="shared" si="7"/>
         <v>5.5919258766043284E-3</v>
       </c>
       <c r="Y52">
-        <f>T52*(T$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>1.6104746524620468E-2</v>
       </c>
       <c r="Z52">
-        <f>U52*(U$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.3190834995453474E-2</v>
       </c>
       <c r="AA52">
-        <f>V52*(V$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.2263201595635329E-2</v>
       </c>
       <c r="AB52">
-        <f>W52*(W$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>1.6029505148857433E-2</v>
       </c>
     </row>
-    <row r="53" spans="17:29">
+    <row r="53" spans="17:30">
       <c r="Q53">
         <v>4</v>
       </c>
@@ -3604,27 +3813,27 @@
         <v>7.6941624714515688E-3</v>
       </c>
       <c r="X53">
-        <f>S53*(S$48*0.2)</f>
+        <f t="shared" si="7"/>
         <v>2.684124420770078E-3</v>
       </c>
       <c r="Y53">
-        <f>T53*(T$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>7.7302783318178251E-3</v>
       </c>
       <c r="Z53">
-        <f>U53*(U$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>1.1131600797817666E-2</v>
       </c>
       <c r="AA53">
-        <f>V53*(V$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>1.068633676590496E-2</v>
       </c>
       <c r="AB53">
-        <f>W53*(W$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>7.6941624714515688E-3</v>
       </c>
     </row>
-    <row r="54" spans="17:29">
+    <row r="54" spans="17:30">
       <c r="Q54">
         <v>5</v>
       </c>
@@ -3647,27 +3856,47 @@
         <v>2.9545583890374033E-3</v>
       </c>
       <c r="X54">
-        <f>S54*(S$48*0.2)</f>
+        <f t="shared" si="7"/>
         <v>1.0307037775757102E-3</v>
       </c>
       <c r="Y54">
-        <f>T54*(T$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.9684268794180455E-3</v>
       </c>
       <c r="Z54">
-        <f>U54*(U$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>4.2745347063619854E-3</v>
       </c>
       <c r="AA54">
-        <f>V54*(V$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>4.1035533181075058E-3</v>
       </c>
       <c r="AB54">
-        <f>W54*(W$48*0.2)</f>
+        <f t="shared" si="8"/>
         <v>2.9545583890374033E-3</v>
       </c>
     </row>
-    <row r="55" spans="17:29">
+    <row r="55" spans="17:30">
+      <c r="S55">
+        <f>SUM(S49:S54)</f>
+        <v>0.15942957206916164</v>
+      </c>
+      <c r="T55">
+        <f>SUM(T49:T54)*2</f>
+        <v>0.45915716755918562</v>
+      </c>
+      <c r="U55">
+        <f>SUM(U49:U54)*3</f>
+        <v>0.66118632128522714</v>
+      </c>
+      <c r="V55">
+        <f>SUM(V49:V54)*4</f>
+        <v>0.63473886843381799</v>
+      </c>
+      <c r="W55">
+        <f>SUM(W49:W54)*5</f>
+        <v>0.45701198527234888</v>
+      </c>
       <c r="AB55" t="s">
         <v>108</v>
       </c>
@@ -3676,7 +3905,11 @@
         <v>2.8458286975436904</v>
       </c>
     </row>
-    <row r="56" spans="17:29">
+    <row r="56" spans="17:30">
+      <c r="W56">
+        <f>SUM(S55:W55)*0.2*6</f>
+        <v>2.8458286975436899</v>
+      </c>
       <c r="AB56" t="s">
         <v>109</v>
       </c>
@@ -3685,16 +3918,16 @@
         <v>2.8458286975436904</v>
       </c>
     </row>
-    <row r="57" spans="17:29">
+    <row r="57" spans="17:30">
       <c r="AB57" t="s">
         <v>110</v>
       </c>
       <c r="AC57">
-        <f>AB36</f>
-        <v>0.54402533346878368</v>
-      </c>
-    </row>
-    <row r="58" spans="17:29">
+        <f>AB42</f>
+        <v>2.6315626159115715E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="17:30">
       <c r="AB58" t="s">
         <v>111</v>
       </c>
@@ -3702,11 +3935,15 @@
         <f>AA33</f>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="59" spans="17:29">
+      <c r="AD58">
+        <f>SUM(AC57:AC58)</f>
+        <v>0.42631562615911572</v>
+      </c>
+    </row>
+    <row r="59" spans="17:30">
       <c r="AC59">
         <f>SUM(AC55:AC58)</f>
-        <v>6.6356827285561648</v>
+        <v>6.1179730212464971</v>
       </c>
     </row>
   </sheetData>
@@ -3725,7 +3962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView topLeftCell="X18" workbookViewId="0">
+    <sheetView topLeftCell="V21" workbookViewId="0">
       <selection activeCell="AD43" sqref="AD43"/>
     </sheetView>
   </sheetViews>
@@ -4703,14 +4940,14 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
       <c r="M16" s="2">
         <v>41611.833333333336</v>
       </c>
@@ -4856,11 +5093,11 @@
         <v>0.9861534547738493</v>
       </c>
       <c r="C18">
-        <f>POISSON(C17,$B$13,FALSE)</f>
+        <f t="shared" ref="C18:H18" si="0">POISSON(C17,$B$13,FALSE)</f>
         <v>0.14660696213035052</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:H18" si="0">POISSON(D17,$B$13,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.28148536729027301</v>
       </c>
       <c r="E18">
@@ -4938,14 +5175,14 @@
       </c>
     </row>
     <row r="19" spans="1:31">
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
       <c r="M19" s="2">
         <v>41630.53125</v>
       </c>
@@ -5243,16 +5480,16 @@
       </c>
     </row>
     <row r="23" spans="1:31">
-      <c r="C23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="M23" s="2">
         <v>41286.625</v>
       </c>
@@ -5395,7 +5632,7 @@
       </c>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B25">
@@ -5496,7 +5733,7 @@
       </c>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -5595,7 +5832,7 @@
       </c>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>2</v>
       </c>
@@ -5694,7 +5931,7 @@
       </c>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>3</v>
       </c>
@@ -5793,7 +6030,7 @@
       </c>
     </row>
     <row r="29" spans="1:31">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>4</v>
       </c>
@@ -5892,7 +6129,7 @@
       </c>
     </row>
     <row r="30" spans="1:31">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30">
         <v>5</v>
       </c>
@@ -6406,7 +6643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -6529,14 +6766,14 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1"/>
@@ -6593,14 +6830,14 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:11">
       <c r="C20">
@@ -6670,16 +6907,16 @@
       <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="C23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:11">
       <c r="C24">
@@ -6708,7 +6945,7 @@
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B25">
@@ -6752,7 +6989,7 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -6794,7 +7031,7 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>2</v>
       </c>
@@ -6836,7 +7073,7 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>3</v>
       </c>
@@ -6878,7 +7115,7 @@
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>4</v>
       </c>
@@ -6920,7 +7157,7 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30">
         <v>5</v>
       </c>
@@ -7157,14 +7394,14 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1"/>
@@ -7196,11 +7433,11 @@
         <v>0.9861534547738493</v>
       </c>
       <c r="C18">
-        <f>POISSON(C17,$B$13,FALSE)</f>
+        <f t="shared" ref="C18:H18" si="0">POISSON(C17,$B$13,FALSE)</f>
         <v>0.14660696213035052</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:H18" si="0">POISSON(D17,$B$13,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.28148536729027301</v>
       </c>
       <c r="E18">
@@ -7221,14 +7458,14 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:11">
       <c r="C20">
@@ -7298,16 +7535,16 @@
       <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="C23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:11">
       <c r="C24">
@@ -7336,7 +7573,7 @@
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B25">
@@ -7380,7 +7617,7 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -7422,7 +7659,7 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>2</v>
       </c>
@@ -7464,7 +7701,7 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>3</v>
       </c>
@@ -7506,7 +7743,7 @@
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>4</v>
       </c>
@@ -7548,7 +7785,7 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30">
         <v>5</v>
       </c>
@@ -7662,24 +7899,1642 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <f>A2/C2</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="J3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f>D4/F4</f>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f>SUM(A4:B4)/(C4*2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="L4">
+        <f>J4/K4</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>D5/F5</f>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f>SUM(A5:B5)/(C5*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="L5">
+        <f>J5/K5</f>
+        <v>1.1428571428571428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="J6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N6" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f>H7/I7</f>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f>SUM(A7:B7)/(C7*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="L7">
+        <f>J7/K7</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="M7">
+        <f>D7/F7</f>
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <f>SUM(A7:B7)/(C7*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="O7">
+        <f>J7/K7</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="P7">
+        <f>A7/C7</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="J8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" t="s">
+        <v>133</v>
+      </c>
+      <c r="N8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O8" t="s">
+        <v>118</v>
+      </c>
+      <c r="P8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8" t="s">
+        <v>117</v>
+      </c>
+      <c r="S8" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" t="s">
+        <v>136</v>
+      </c>
+      <c r="U8" t="s">
+        <v>117</v>
+      </c>
+      <c r="V8" t="s">
+        <v>137</v>
+      </c>
+      <c r="W8" t="s">
+        <v>116</v>
+      </c>
+      <c r="X8" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f>E9/F9</f>
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <f>SUM($A9:$B9)/($C9*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="L9">
+        <f>J9/K9</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="M9">
+        <f>G9/I9</f>
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <f>SUM(A9:B9)/(C9*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="O9">
+        <f>M9/N9</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="P9">
+        <f>B9/C9</f>
+        <v>1.5</v>
+      </c>
+      <c r="Q9">
+        <f>H9/I9</f>
+        <v>1.5</v>
+      </c>
+      <c r="R9">
+        <f>SUM($A9:$B9)/($C9*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="S9">
+        <f>Q9/R9</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="T9">
+        <f>D9/F9</f>
+        <v>1.5</v>
+      </c>
+      <c r="U9">
+        <f>SUM($A9:$B9)/($C9*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="V9">
+        <f>T9/U9</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="W9">
+        <f>A9/C9</f>
+        <v>2</v>
+      </c>
+      <c r="X9">
+        <f>W9*V9*S9</f>
+        <v>1.4693877551020407</v>
+      </c>
+      <c r="Y9">
+        <f>P9*O9*L9</f>
+        <v>1.9591836734693875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f>E10/F10</f>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f>SUM(A10:B10)/(C10*2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L10">
+        <f>J10/K10</f>
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <f>G10/I10</f>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>SUM(A10:B10)/(C10*2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="O10">
+        <f>M10/N10</f>
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <f>B10/C10</f>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10:Q13" si="0">H10/I10</f>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ref="R10:R14" si="1">SUM($A10:$B10)/($C10*2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ref="S10:S12" si="2">Q10/R10</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ref="T10:T13" si="3">D10/F10</f>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ref="U10:U14" si="4">SUM($A10:$B10)/($C10*2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ref="V10:V12" si="5">T10/U10</f>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f t="shared" ref="W10:W12" si="6">A10/C10</f>
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <f t="shared" ref="X10:X12" si="7">W10*V10*S10</f>
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <f>P10*O10*L10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f>E11/F11</f>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f>SUM(A11:B11)/(C11*2)</f>
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <f>J11/K11</f>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f>G11/I11</f>
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f>SUM(A11:B11)/(C11*2)</f>
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <f>M11/N11</f>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <f>B11/C11</f>
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <f>P11*O11*L11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f>E12/F12</f>
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <f>SUM(A12:B12)/(C12*2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="L12">
+        <f>J12/K12</f>
+        <v>1.2</v>
+      </c>
+      <c r="M12">
+        <f>G12/I12</f>
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <f>SUM(A12:B12)/(C12*2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="O12">
+        <f>M12/N12</f>
+        <v>1.2</v>
+      </c>
+      <c r="P12">
+        <f>B12/C12</f>
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="7"/>
+        <v>1.9200000000000004</v>
+      </c>
+      <c r="Y12">
+        <f>P12*O12*L12</f>
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <f>E13/F13</f>
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f>SUM(A13:B13)/(C13*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="L13">
+        <f>J13/K13</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="M13">
+        <f>G13/I13</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="N13">
+        <f>SUM(A13:B13)/(C13*2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="O13">
+        <f>M13/N13</f>
+        <v>1.3333333333333335</v>
+      </c>
+      <c r="P13">
+        <f>B13/C13</f>
+        <v>1.5</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ref="Q13" si="8">H13/I13</f>
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ref="S13" si="9">Q13/R13</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ref="T13" si="10">D13/F13</f>
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="4"/>
+        <v>1.75</v>
+      </c>
+      <c r="V13">
+        <f t="shared" ref="V13" si="11">T13/U13</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="W13">
+        <f t="shared" ref="W13" si="12">A13/C13</f>
+        <v>2</v>
+      </c>
+      <c r="X13">
+        <f t="shared" ref="X13" si="13">W13*V13*S13</f>
+        <v>1.3061224489795917</v>
+      </c>
+      <c r="Y13">
+        <f>P13*O13*L13</f>
+        <v>2.2857142857142856</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <f>(A14/C14)*((D14/F14)/(SUM($A14:$B14)/($C14*2)))*((H14/I14)/(SUM($A14:$B14)/($C14*2)))</f>
+        <v>1.3061224489795917</v>
+      </c>
+      <c r="Y14">
+        <f>(B14/C14)*((G14/I14)/(SUM(A14:B14)/(C14*2)))*((E14/F14)/(SUM(A14:B14)/(C14*2)))</f>
+        <v>2.2857142857142856</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="7"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1.3414999999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.73170000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1.2195</v>
+      </c>
+      <c r="F3">
+        <v>1.0975999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>0.48780000000000001</v>
+      </c>
+      <c r="F4">
+        <v>1.4634</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1.2195</v>
+      </c>
+      <c r="F5">
+        <v>0.60980000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>0.60980000000000001</v>
+      </c>
+      <c r="F6">
+        <v>1.3414999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>1.8292999999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.85370000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>0.48780000000000001</v>
+      </c>
+      <c r="F8">
+        <v>1.0975999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="F9">
+        <v>0.60980000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="F10">
+        <v>1.8292999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>0.85370000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.73170000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>1.0975999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.85370000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>0.3659</v>
+      </c>
+      <c r="F13">
+        <v>0.97560000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>0.85370000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.73170000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1.8292999999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.24390000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>1.4634</v>
+      </c>
+      <c r="F16">
+        <v>0.73170000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="F17">
+        <v>1.2195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="F18">
+        <v>1.0975999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>0.60980000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.97560000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>1.0975999999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.73170000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="F21">
+        <v>2.0731999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22">
+        <v>1.6167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23">
+        <v>1.1167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" t="s">
+        <v>172</v>
+      </c>
+      <c r="E27" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I27" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28">
+        <v>97</v>
+      </c>
+      <c r="C28">
+        <v>67</v>
+      </c>
+      <c r="D28">
+        <v>60</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>6</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <f>(B28/D28)*((E28/G28)/(SUM($B28:$C28)/($D28*2)))*((I28/J28)/(SUM($B28:$C28)/($D28*2)))</f>
+        <v>2.5966686496133256</v>
+      </c>
+      <c r="L28">
+        <f>(C28/D28)*((H28/J28)/(SUM(B28:C28)/(D28*2)))*((F28/G28)/(SUM(B28:C28)/(D28*2)))</f>
+        <v>0.97650208209399181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29">
+        <v>97</v>
+      </c>
+      <c r="C29">
+        <v>67</v>
+      </c>
+      <c r="D29">
+        <v>60</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K36" si="0">(B29/D29)*((E29/G29)/(SUM($B29:$C29)/($D29*2)))*((I29/J29)/(SUM($B29:$C29)/($D29*2)))</f>
+        <v>0.86555621653777504</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L36" si="1">(C29/D29)*((H29/J29)/(SUM(B29:C29)/(D29*2)))*((F29/G29)/(SUM(B29:C29)/(D29*2)))</f>
+        <v>0.76867510835387109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30">
+        <v>97</v>
+      </c>
+      <c r="C30">
+        <v>67</v>
+      </c>
+      <c r="D30">
+        <v>60</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+      <c r="J30">
+        <v>7</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>1.5456361009603126</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0.91102235064162473</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31">
+        <v>97</v>
+      </c>
+      <c r="C31">
+        <v>67</v>
+      </c>
+      <c r="D31">
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>17</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>9</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>1.4838106569219003</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0.9679612475567263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32">
+        <v>97</v>
+      </c>
+      <c r="C32">
+        <v>67</v>
+      </c>
+      <c r="D32">
+        <v>60</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>6</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>12</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>2.8851873884592503</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>0.59785841760856628</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33">
+        <v>97</v>
+      </c>
+      <c r="C33">
+        <v>67</v>
+      </c>
+      <c r="D33">
+        <v>60</v>
+      </c>
+      <c r="K33" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L33" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>178</v>
+      </c>
+      <c r="B34">
+        <v>97</v>
+      </c>
+      <c r="C34">
+        <v>67</v>
+      </c>
+      <c r="D34">
+        <v>60</v>
+      </c>
+      <c r="K34" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L34" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>179</v>
+      </c>
+      <c r="B35">
+        <v>97</v>
+      </c>
+      <c r="C35">
+        <v>67</v>
+      </c>
+      <c r="D35">
+        <v>60</v>
+      </c>
+      <c r="K35" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36">
+        <v>97</v>
+      </c>
+      <c r="C36">
+        <v>67</v>
+      </c>
+      <c r="D36">
+        <v>60</v>
+      </c>
+      <c r="K36" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L36" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7688,7 +9543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView topLeftCell="W16" workbookViewId="0">
+    <sheetView topLeftCell="W19" workbookViewId="0">
       <selection activeCell="AD43" sqref="AD43"/>
     </sheetView>
   </sheetViews>
@@ -8665,14 +10520,14 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
       <c r="M16" s="2">
         <v>41616.625</v>
       </c>
@@ -8818,11 +10673,11 @@
         <v>0.9861534547738493</v>
       </c>
       <c r="C18">
-        <f>POISSON(C17,$B$13,FALSE)</f>
+        <f t="shared" ref="C18:H18" si="0">POISSON(C17,$B$13,FALSE)</f>
         <v>0.14660696213035052</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:H18" si="0">POISSON(D17,$B$13,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.28148536729027301</v>
       </c>
       <c r="E18">
@@ -8900,14 +10755,14 @@
       </c>
     </row>
     <row r="19" spans="1:31">
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
       <c r="M19" s="2">
         <v>41630.625</v>
       </c>
@@ -9205,16 +11060,16 @@
       </c>
     </row>
     <row r="23" spans="1:31">
-      <c r="C23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="M23" s="2">
         <v>41286.625</v>
       </c>
@@ -9357,7 +11212,7 @@
       </c>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B25">
@@ -9458,7 +11313,7 @@
       </c>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -9557,7 +11412,7 @@
       </c>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>2</v>
       </c>
@@ -9656,7 +11511,7 @@
       </c>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>3</v>
       </c>
@@ -9755,7 +11610,7 @@
       </c>
     </row>
     <row r="29" spans="1:31">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>4</v>
       </c>
@@ -9854,7 +11709,7 @@
       </c>
     </row>
     <row r="30" spans="1:31">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Gave player knowledge of their team, now reference is bi-directional.  Not sure if this is a brilliant idea.
</commit_message>
<xml_diff>
--- a/data/poission.xlsx
+++ b/data/poission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="20940" windowHeight="10110" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20940" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Figueroa" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="190">
   <si>
     <t>Wigan</t>
   </si>
@@ -564,6 +564,33 @@
   </si>
   <si>
     <t>sunderland man united</t>
+  </si>
+  <si>
+    <t>expected home</t>
+  </si>
+  <si>
+    <t>expected away</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>correct score</t>
+  </si>
+  <si>
+    <t>correct result</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>correct goals</t>
+  </si>
+  <si>
+    <t>standard deviation of goals</t>
   </si>
 </sst>
 </file>
@@ -620,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
@@ -637,6 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3306,6 +3334,14 @@
         <f>SUM(C26:C30,D27:D30,E28:E30,F29:F30,G29)</f>
         <v>0.24339187734248208</v>
       </c>
+      <c r="H34">
+        <f>C18*4</f>
+        <v>0.58642784852140206</v>
+      </c>
+      <c r="I34">
+        <f>(C18*4)+(SUM(E18:F18)*-1)+(SUM(G18:H18)*-2)</f>
+        <v>-8.6523839923243334E-2</v>
+      </c>
       <c r="U34">
         <f>CORREL(T2:T32, Z2:Z32)</f>
         <v>0.25820183151655701</v>
@@ -3323,6 +3359,14 @@
         <f>SUM(C25:C30)</f>
         <v>5.5357490301792232E-2</v>
       </c>
+      <c r="I35">
+        <f>(SUM(E18:F18))</f>
+        <v>0.44317056226180596</v>
+      </c>
+      <c r="J35">
+        <f>I35*-1</f>
+        <v>-0.44317056226180596</v>
+      </c>
     </row>
     <row r="36" spans="1:30">
       <c r="A36" t="s">
@@ -3331,6 +3375,18 @@
       <c r="B36">
         <f>SUM(C25,D26,E27,F28,G29,H30)</f>
         <v>0.17160999344858832</v>
+      </c>
+      <c r="I36">
+        <f>SUM(G18:H18)</f>
+        <v>0.11489056309141972</v>
+      </c>
+      <c r="J36">
+        <f>I36*-2</f>
+        <v>-0.22978112618283944</v>
+      </c>
+      <c r="K36">
+        <f>J36+J35+H34</f>
+        <v>-8.6523839923243306E-2</v>
       </c>
       <c r="R36" s="4">
         <v>8.2297470490201394E-3</v>
@@ -3371,6 +3427,24 @@
       <c r="B37" t="s">
         <v>22</v>
       </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0.99</v>
+      </c>
+      <c r="G37">
+        <f>POISSON(E37-1,F37,FALSE)</f>
+        <v>0.3715766910220516</v>
+      </c>
+      <c r="H37">
+        <f>POISSON(E37, F37, FALSE)</f>
+        <v>0.36786092411183108</v>
+      </c>
+      <c r="I37">
+        <f>POISSON(E37+1,F37,FALSE)</f>
+        <v>0.18209115743535639</v>
+      </c>
       <c r="R37">
         <v>1.5801114334118668E-2</v>
       </c>
@@ -3398,6 +3472,24 @@
       </c>
     </row>
     <row r="38" spans="1:30">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f>POISSON(E38-1,F38,FALSE)</f>
+        <v>0.36787944117144911</v>
+      </c>
+      <c r="H38">
+        <f>POISSON(E38, F38, FALSE)</f>
+        <v>0.36787944117144911</v>
+      </c>
+      <c r="I38">
+        <f>POISSON(E38+1,F38,FALSE)</f>
+        <v>0.18393972058572455</v>
+      </c>
       <c r="R38" s="5">
         <v>1.5169069760753925E-2</v>
       </c>
@@ -3420,6 +3512,24 @@
       <c r="Y38" s="5"/>
     </row>
     <row r="39" spans="1:30">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1.01</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ref="G39:G48" si="7">POISSON(E39-1,F39,FALSE)</f>
+        <v>0.36421897957153127</v>
+      </c>
+      <c r="H39">
+        <f>POISSON(E39, F39, FALSE)</f>
+        <v>0.36786116936724655</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:I48" si="8">POISSON(E39+1,F39,FALSE)</f>
+        <v>0.18576989053045953</v>
+      </c>
       <c r="R39" s="5">
         <v>9.7082046468825144E-3</v>
       </c>
@@ -3453,6 +3563,24 @@
       </c>
     </row>
     <row r="40" spans="1:30">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1.2</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="7"/>
+        <v>0.30119421191220819</v>
+      </c>
+      <c r="H40">
+        <f>POISSON(E40, F40, FALSE)</f>
+        <v>0.36143305429464984</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="8"/>
+        <v>0.21685983257678987</v>
+      </c>
       <c r="R40" s="6">
         <v>4.6599382305036073E-3</v>
       </c>
@@ -3475,6 +3603,24 @@
       <c r="Y40" s="6"/>
     </row>
     <row r="41" spans="1:30">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1.3</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="7"/>
+        <v>0.27253179303401398</v>
+      </c>
+      <c r="H41">
+        <f>POISSON(E41, F41, FALSE)</f>
+        <v>0.35429133094421822</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="8"/>
+        <v>0.23028936511374185</v>
+      </c>
       <c r="R41" s="6">
         <v>1.7894162805133858E-3</v>
       </c>
@@ -3508,6 +3654,24 @@
       </c>
     </row>
     <row r="42" spans="1:30">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1.4</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="7"/>
+        <v>0.2465969639416109</v>
+      </c>
+      <c r="H42">
+        <f>POISSON(E42, F42, FALSE)</f>
+        <v>0.34523574951825525</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="8"/>
+        <v>0.24166502466277867</v>
+      </c>
       <c r="R42">
         <f>SUM(R36:R41)</f>
         <v>5.5357490301792232E-2</v>
@@ -3534,6 +3698,24 @@
       </c>
     </row>
     <row r="43" spans="1:30">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1.5</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="7"/>
+        <v>0.22313016014843082</v>
+      </c>
+      <c r="H43">
+        <f>POISSON(E43, F43, FALSE)</f>
+        <v>0.33469524022264624</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="8"/>
+        <v>0.25102143016698469</v>
+      </c>
       <c r="R43">
         <f>R42*4</f>
         <v>0.22142996120716893</v>
@@ -3559,6 +3741,24 @@
       </c>
     </row>
     <row r="44" spans="1:30">
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1.6</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="7"/>
+        <v>0.20189651799465819</v>
+      </c>
+      <c r="H44">
+        <f>POISSON(E44, F44, FALSE)</f>
+        <v>0.32303442879145311</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="8"/>
+        <v>0.25842754303316251</v>
+      </c>
       <c r="U44">
         <f>SUM(R43:U43)</f>
         <v>-0.22854406300083294</v>
@@ -3569,6 +3769,24 @@
       </c>
     </row>
     <row r="45" spans="1:30">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1.7</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="7"/>
+        <v>0.18268352405273522</v>
+      </c>
+      <c r="H45">
+        <f>POISSON(E45, F45, FALSE)</f>
+        <v>0.31056199088964986</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="8"/>
+        <v>0.26397769225620238</v>
+      </c>
       <c r="T45">
         <f>SUM(T36:T41)</f>
         <v>0.22957858377959281</v>
@@ -3579,6 +3797,24 @@
       </c>
     </row>
     <row r="46" spans="1:30">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1.8</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="7"/>
+        <v>0.16529888822158814</v>
+      </c>
+      <c r="H46">
+        <f>POISSON(E46, F46, FALSE)</f>
+        <v>0.29753799879885862</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="8"/>
+        <v>0.26778419891897276</v>
+      </c>
       <c r="T46">
         <f>T45*-1</f>
         <v>-0.22957858377959281</v>
@@ -3589,6 +3825,24 @@
       </c>
     </row>
     <row r="47" spans="1:30">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>1.99</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="7"/>
+        <v>0.13669542544552463</v>
+      </c>
+      <c r="H47">
+        <f>POISSON(E47, F47, FALSE)</f>
+        <v>0.27202389663659404</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="8"/>
+        <v>0.27066377715341106</v>
+      </c>
       <c r="T47">
         <f>T46+R43</f>
         <v>-8.1486225724238803E-3</v>
@@ -3618,7 +3872,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="17:30">
+    <row r="49" spans="16:30">
+      <c r="P49">
+        <f>SUM(R49:W49)</f>
+        <v>0.13600633336719592</v>
+      </c>
       <c r="Q49">
         <v>0</v>
       </c>
@@ -3641,7 +3899,7 @@
         <v>1.3588379880148507E-2</v>
       </c>
       <c r="X49">
-        <f t="shared" ref="X49:X54" si="7">S49*(S$48*0.2)</f>
+        <f>S49*(S$48*0.2)</f>
         <v>4.7403343002356008E-3</v>
       </c>
       <c r="Y49">
@@ -3661,7 +3919,7 @@
         <v>1.3588379880148507E-2</v>
       </c>
     </row>
-    <row r="50" spans="17:30">
+    <row r="50" spans="16:30">
       <c r="Q50">
         <v>1</v>
       </c>
@@ -3684,27 +3942,27 @@
         <v>2.6089689369885136E-2</v>
       </c>
       <c r="X50">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="X49:X54" si="9">S50*(S$48*0.2)</f>
         <v>9.1014418564523535E-3</v>
       </c>
       <c r="Y50">
-        <f t="shared" ref="Y50:AB54" si="8">T50*(T$48*0.2)</f>
+        <f t="shared" ref="Y50:AB54" si="10">T50*(T$48*0.2)</f>
         <v>2.6212152546582781E-2</v>
       </c>
       <c r="Z50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.7745499667079199E-2</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6235679680396031E-2</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.6089689369885136E-2</v>
       </c>
     </row>
-    <row r="51" spans="17:30">
+    <row r="51" spans="16:30">
       <c r="Q51">
         <v>2</v>
       </c>
@@ -3727,27 +3985,27 @@
         <v>2.5046101795089735E-2</v>
       </c>
       <c r="X51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8.7373841821942622E-3</v>
       </c>
       <c r="Y51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.5163666444719474E-2</v>
       </c>
       <c r="Z51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6235679680396045E-2</v>
       </c>
       <c r="AA51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.4786252493180202E-2</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.5046101795089735E-2</v>
       </c>
     </row>
-    <row r="52" spans="17:30">
+    <row r="52" spans="16:30">
       <c r="Q52">
         <v>3</v>
       </c>
@@ -3770,27 +4028,27 @@
         <v>1.6029505148857433E-2</v>
       </c>
       <c r="X52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.5919258766043284E-3</v>
       </c>
       <c r="Y52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6104746524620468E-2</v>
       </c>
       <c r="Z52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.3190834995453474E-2</v>
       </c>
       <c r="AA52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.2263201595635329E-2</v>
       </c>
       <c r="AB52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6029505148857433E-2</v>
       </c>
     </row>
-    <row r="53" spans="17:30">
+    <row r="53" spans="16:30">
       <c r="Q53">
         <v>4</v>
       </c>
@@ -3813,27 +4071,27 @@
         <v>7.6941624714515688E-3</v>
       </c>
       <c r="X53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.684124420770078E-3</v>
       </c>
       <c r="Y53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.7302783318178251E-3</v>
       </c>
       <c r="Z53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.1131600797817666E-2</v>
       </c>
       <c r="AA53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.068633676590496E-2</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.6941624714515688E-3</v>
       </c>
     </row>
-    <row r="54" spans="17:30">
+    <row r="54" spans="16:30">
       <c r="Q54">
         <v>5</v>
       </c>
@@ -3856,27 +4114,27 @@
         <v>2.9545583890374033E-3</v>
       </c>
       <c r="X54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.0307037775757102E-3</v>
       </c>
       <c r="Y54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.9684268794180455E-3</v>
       </c>
       <c r="Z54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.2745347063619854E-3</v>
       </c>
       <c r="AA54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1035533181075058E-3</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.9545583890374033E-3</v>
       </c>
     </row>
-    <row r="55" spans="17:30">
+    <row r="55" spans="16:30">
       <c r="S55">
         <f>SUM(S49:S54)</f>
         <v>0.15942957206916164</v>
@@ -3905,7 +4163,7 @@
         <v>2.8458286975436904</v>
       </c>
     </row>
-    <row r="56" spans="17:30">
+    <row r="56" spans="16:30">
       <c r="W56">
         <f>SUM(S55:W55)*0.2*6</f>
         <v>2.8458286975436899</v>
@@ -3918,7 +4176,7 @@
         <v>2.8458286975436904</v>
       </c>
     </row>
-    <row r="57" spans="17:30">
+    <row r="57" spans="16:30">
       <c r="AB57" t="s">
         <v>110</v>
       </c>
@@ -3927,7 +4185,7 @@
         <v>2.6315626159115715E-2</v>
       </c>
     </row>
-    <row r="58" spans="17:30">
+    <row r="58" spans="16:30">
       <c r="AB58" t="s">
         <v>111</v>
       </c>
@@ -3940,7 +4198,7 @@
         <v>0.42631562615911572</v>
       </c>
     </row>
-    <row r="59" spans="17:30">
+    <row r="59" spans="16:30">
       <c r="AC59">
         <f>SUM(AC55:AC58)</f>
         <v>6.1179730212464971</v>
@@ -3962,8 +4220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView topLeftCell="V21" workbookViewId="0">
-      <selection activeCell="AD43" sqref="AD43"/>
+    <sheetView topLeftCell="K19" workbookViewId="0">
+      <selection activeCell="AD44" sqref="AD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6335,6 +6593,14 @@
         <f>SUM(C26:C30,D27:D30,E28:E30,F29:F30,G29)</f>
         <v>0.24339187734248208</v>
       </c>
+      <c r="H34">
+        <f>C18*4</f>
+        <v>0.58642784852140206</v>
+      </c>
+      <c r="I34">
+        <f>(C18*4)+(SUM(E18:F18)*-1)+(SUM(G18:H18)*-2)</f>
+        <v>-8.6523839923243334E-2</v>
+      </c>
       <c r="U34">
         <f>CORREL(T2:T32, Z2:Z32)</f>
         <v>0.14652413961158087</v>
@@ -6352,6 +6618,14 @@
         <f>SUM(C25:C30)</f>
         <v>5.5357490301792232E-2</v>
       </c>
+      <c r="I35">
+        <f>(SUM(E18:F18))</f>
+        <v>0.44317056226180596</v>
+      </c>
+      <c r="J35">
+        <f>I35*-1</f>
+        <v>-0.44317056226180596</v>
+      </c>
     </row>
     <row r="36" spans="1:30">
       <c r="A36" t="s">
@@ -6360,6 +6634,18 @@
       <c r="B36">
         <f>SUM(C25,D26,E27,F28,G29,H30)</f>
         <v>0.17160999344858832</v>
+      </c>
+      <c r="I36">
+        <f>SUM(G18:H18)</f>
+        <v>0.11489056309141972</v>
+      </c>
+      <c r="J36">
+        <f>I36*-2</f>
+        <v>-0.22978112618283944</v>
+      </c>
+      <c r="K36">
+        <f>J36+J35+H34</f>
+        <v>-8.6523839923243306E-2</v>
       </c>
       <c r="R36" s="4">
         <v>8.2297470490201394E-3</v>
@@ -6529,11 +6815,11 @@
         <v>0.10658323450330624</v>
       </c>
       <c r="AA41" s="6">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AB41">
         <f>Z41*AA41</f>
-        <v>-0.10658323450330624</v>
+        <v>-0.21316646900661249</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -6559,7 +6845,7 @@
       </c>
       <c r="AB42">
         <f>SUM(AB36:AB41)</f>
-        <v>2.6315626159115715E-2</v>
+        <v>-8.0267608344190527E-2</v>
       </c>
     </row>
     <row r="43" spans="1:30">
@@ -6583,8 +6869,8 @@
         <v>81</v>
       </c>
       <c r="AD43">
-        <f>AB42+Z34+AA33</f>
-        <v>1.626315624959116</v>
+        <f>K36+Z34+AA33</f>
+        <v>1.5134761588767569</v>
       </c>
     </row>
     <row r="44" spans="1:30">
@@ -8746,15 +9032,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9077,7 +9367,7 @@
         <v>0.73170000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
         <v>157</v>
       </c>
@@ -9097,7 +9387,7 @@
         <v>1.2195</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -9117,7 +9407,7 @@
         <v>1.0975999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -9137,7 +9427,7 @@
         <v>0.97560000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -9157,7 +9447,7 @@
         <v>0.73170000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>161</v>
       </c>
@@ -9177,7 +9467,7 @@
         <v>2.0731999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -9185,7 +9475,7 @@
         <v>1.6167</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -9193,7 +9483,7 @@
         <v>1.1167</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -9201,7 +9491,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
         <v>170</v>
       </c>
@@ -9209,7 +9499,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
         <v>171</v>
       </c>
@@ -9217,7 +9507,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:24">
       <c r="B27" t="s">
         <v>112</v>
       </c>
@@ -9245,8 +9535,50 @@
       <c r="J27" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="K27" t="s">
+        <v>181</v>
+      </c>
+      <c r="L27" t="s">
+        <v>182</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <v>4</v>
+      </c>
+      <c r="R27">
+        <v>5</v>
+      </c>
+      <c r="S27" t="s">
+        <v>183</v>
+      </c>
+      <c r="T27" t="s">
+        <v>184</v>
+      </c>
+      <c r="U27" t="s">
+        <v>185</v>
+      </c>
+      <c r="V27" t="s">
+        <v>186</v>
+      </c>
+      <c r="W27" t="s">
+        <v>188</v>
+      </c>
+      <c r="X27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
         <v>164</v>
       </c>
@@ -9285,50 +9617,78 @@
         <f>(C28/D28)*((H28/J28)/(SUM(B28:C28)/(D28*2)))*((F28/G28)/(SUM(B28:C28)/(D28*2)))</f>
         <v>0.97650208209399181</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
+      <c r="M28">
+        <f>POISSON(M$27,$K28,FALSE)</f>
+        <v>7.4521422126082218E-2</v>
+      </c>
+      <c r="N28">
+        <f>POISSON(N$27,$K28,FALSE)</f>
+        <v>0.19350744055939853</v>
+      </c>
+      <c r="O28">
+        <f>POISSON(O$27,$K28,FALSE)</f>
+        <v>0.25123735218375209</v>
+      </c>
+      <c r="P28">
+        <f>POISSON(P$27,$K28,FALSE)</f>
+        <v>0.21746005200913701</v>
+      </c>
+      <c r="Q28">
+        <f>POISSON(Q$27,$K28,FALSE)</f>
+        <v>0.14116792489885235</v>
+      </c>
+      <c r="R28">
+        <f>POISSON(R$27,$K28,FALSE)</f>
+        <v>7.3313264983163651E-2</v>
+      </c>
+      <c r="S28">
+        <v>2</v>
+      </c>
+      <c r="T28">
+        <v>3</v>
+      </c>
+      <c r="V28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="M29">
+        <f>POISSON(M$27,$L28,FALSE)</f>
+        <v>0.37662620499014893</v>
+      </c>
+      <c r="N29">
+        <f>POISSON(N$27,$L28,FALSE)</f>
+        <v>0.36777627334403901</v>
+      </c>
+      <c r="O29">
+        <f>POISSON(O$27,$L28,FALSE)</f>
+        <v>0.17956714833261159</v>
+      </c>
+      <c r="P29">
+        <f>POISSON(P$27,$L28,FALSE)</f>
+        <v>5.8449231407491961E-2</v>
+      </c>
+      <c r="Q29">
+        <f>POISSON(Q$27,$L28,FALSE)</f>
+        <v>1.4268949041552358E-2</v>
+      </c>
+      <c r="R29">
+        <f>POISSON(R$27,$L28,FALSE)</f>
+        <v>2.7867316896737892E-3</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="V29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="A30" t="s">
         <v>173</v>
-      </c>
-      <c r="B29">
-        <v>97</v>
-      </c>
-      <c r="C29">
-        <v>67</v>
-      </c>
-      <c r="D29">
-        <v>60</v>
-      </c>
-      <c r="E29">
-        <v>7</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
-      </c>
-      <c r="G29">
-        <v>7</v>
-      </c>
-      <c r="H29">
-        <v>9</v>
-      </c>
-      <c r="I29">
-        <v>6</v>
-      </c>
-      <c r="J29">
-        <v>6</v>
-      </c>
-      <c r="K29">
-        <f t="shared" ref="K29:K36" si="0">(B29/D29)*((E29/G29)/(SUM($B29:$C29)/($D29*2)))*((I29/J29)/(SUM($B29:$C29)/($D29*2)))</f>
-        <v>0.86555621653777504</v>
-      </c>
-      <c r="L29">
-        <f t="shared" ref="L29:L36" si="1">(C29/D29)*((H29/J29)/(SUM(B29:C29)/(D29*2)))*((F29/G29)/(SUM(B29:C29)/(D29*2)))</f>
-        <v>0.76867510835387109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" t="s">
-        <v>174</v>
       </c>
       <c r="B30">
         <v>97</v>
@@ -9340,202 +9700,889 @@
         <v>60</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>9</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+      <c r="J30">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ref="K30:K44" si="0">(B30/D30)*((E30/G30)/(SUM($B30:$C30)/($D30*2)))*((I30/J30)/(SUM($B30:$C30)/($D30*2)))</f>
+        <v>0.86555621653777504</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ref="L30:L44" si="1">(C30/D30)*((H30/J30)/(SUM(B30:C30)/(D30*2)))*((F30/G30)/(SUM(B30:C30)/(D30*2)))</f>
+        <v>0.76867510835387109</v>
+      </c>
+      <c r="M30">
+        <f>POISSON(M$27,$K30,FALSE)</f>
+        <v>0.42081742191021959</v>
+      </c>
+      <c r="N30">
+        <f>POISSON(N$27,$K30,FALSE)</f>
+        <v>0.36424113556179022</v>
+      </c>
+      <c r="O30">
+        <f>POISSON(O$27,$K30,FALSE)</f>
+        <v>0.15763558960214299</v>
+      </c>
+      <c r="P30">
+        <f>POISSON(P$27,$K30,FALSE)</f>
+        <v>4.5480821509244103E-2</v>
+      </c>
+      <c r="Q30">
+        <f>POISSON(Q$27,$K30,FALSE)</f>
+        <v>9.8415519476427963E-3</v>
+      </c>
+      <c r="R30">
+        <f>POISSON(R$27,$K30,FALSE)</f>
+        <v>1.7036832937323339E-3</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="M31">
+        <f>POISSON(M$27,$L30,FALSE)</f>
+        <v>0.46362691700919872</v>
+      </c>
+      <c r="N31">
+        <f>POISSON(N$27,$L30,FALSE)</f>
+        <v>0.35637847066781703</v>
+      </c>
+      <c r="O31">
+        <f>POISSON(O$27,$L30,FALSE)</f>
+        <v>0.13696962977778557</v>
+      </c>
+      <c r="P31">
+        <f>POISSON(P$27,$L30,FALSE)</f>
+        <v>3.5095048336876308E-2</v>
+      </c>
+      <c r="Q31">
+        <f>POISSON(Q$27,$L30,FALSE)</f>
+        <v>6.7441725207581854E-3</v>
+      </c>
+      <c r="R31">
+        <f>POISSON(R$27,$L30,FALSE)</f>
+        <v>1.0368155086301995E-3</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="A32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32">
+        <v>97</v>
+      </c>
+      <c r="C32">
+        <v>67</v>
+      </c>
+      <c r="D32">
+        <v>60</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
         <v>8</v>
       </c>
-      <c r="G30">
+      <c r="G32">
         <v>6</v>
       </c>
-      <c r="H30">
+      <c r="H32">
         <v>8</v>
       </c>
-      <c r="I30">
+      <c r="I32">
         <v>15</v>
       </c>
-      <c r="J30">
+      <c r="J32">
         <v>7</v>
       </c>
-      <c r="K30">
+      <c r="K32">
         <f t="shared" si="0"/>
         <v>1.5456361009603126</v>
       </c>
-      <c r="L30">
+      <c r="L32">
         <f t="shared" si="1"/>
         <v>0.91102235064162473</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
+      <c r="M32">
+        <f>POISSON(M$27,$K32,FALSE)</f>
+        <v>0.21317622648323414</v>
+      </c>
+      <c r="N32">
+        <f>POISSON(N$27,$K32,FALSE)</f>
+        <v>0.32949287151897855</v>
+      </c>
+      <c r="O32">
+        <f>POISSON(O$27,$K32,FALSE)</f>
+        <v>0.25463803861440559</v>
+      </c>
+      <c r="P32">
+        <f>POISSON(P$27,$K32,FALSE)</f>
+        <v>0.13119258172005047</v>
+      </c>
+      <c r="Q32">
+        <f>POISSON(Q$27,$K32,FALSE)</f>
+        <v>5.0693997621173992E-2</v>
+      </c>
+      <c r="R32">
+        <f>POISSON(R$27,$K32,FALSE)</f>
+        <v>1.5670894565056544E-2</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="M33">
+        <f>POISSON(M$27,$L32,FALSE)</f>
+        <v>0.40211291342258626</v>
+      </c>
+      <c r="N33">
+        <f>POISSON(N$27,$L32,FALSE)</f>
+        <v>0.36633385160959669</v>
+      </c>
+      <c r="O33">
+        <f>POISSON(O$27,$L32,FALSE)</f>
+        <v>0.16686916330648743</v>
+      </c>
+      <c r="P33">
+        <f>POISSON(P$27,$L32,FALSE)</f>
+        <v>5.0673845801692444E-2</v>
+      </c>
+      <c r="Q33">
+        <f>POISSON(Q$27,$L32,FALSE)</f>
+        <v>1.154125152957727E-2</v>
+      </c>
+      <c r="R33">
+        <f>POISSON(R$27,$L32,FALSE)</f>
+        <v>2.102867619564346E-3</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" t="s">
         <v>175</v>
       </c>
-      <c r="B31">
+      <c r="B34">
         <v>97</v>
       </c>
-      <c r="C31">
+      <c r="C34">
         <v>67</v>
       </c>
-      <c r="D31">
+      <c r="D34">
         <v>60</v>
       </c>
-      <c r="E31">
+      <c r="E34">
         <v>8</v>
       </c>
-      <c r="F31">
+      <c r="F34">
         <v>17</v>
       </c>
-      <c r="G31">
+      <c r="G34">
         <v>6</v>
       </c>
-      <c r="H31">
+      <c r="H34">
         <v>4</v>
       </c>
-      <c r="I31">
+      <c r="I34">
         <v>9</v>
       </c>
-      <c r="J31">
+      <c r="J34">
         <v>7</v>
       </c>
-      <c r="K31">
+      <c r="K34">
         <f t="shared" si="0"/>
         <v>1.4838106569219003</v>
       </c>
-      <c r="L31">
+      <c r="L34">
         <f t="shared" si="1"/>
         <v>0.9679612475567263</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" t="s">
+      <c r="M34">
+        <f>POISSON(M$27,$K34,FALSE)</f>
+        <v>0.22677188992902145</v>
+      </c>
+      <c r="N34">
+        <f>POISSON(N$27,$K34,FALSE)</f>
+        <v>0.3364865469670022</v>
+      </c>
+      <c r="O34">
+        <f>POISSON(O$27,$K34,FALSE)</f>
+        <v>0.24964116215024471</v>
+      </c>
+      <c r="P34">
+        <f>POISSON(P$27,$K34,FALSE)</f>
+        <v>0.12347340560163374</v>
+      </c>
+      <c r="Q34">
+        <f>POISSON(Q$27,$K34,FALSE)</f>
+        <v>4.5802788769536099E-2</v>
+      </c>
+      <c r="R34">
+        <f>POISSON(R$27,$K34,FALSE)</f>
+        <v>1.3592533218596079E-2</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>2</v>
+      </c>
+      <c r="V34" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="M35">
+        <f>POISSON(M$27,$L34,FALSE)</f>
+        <v>0.37985668294071917</v>
+      </c>
+      <c r="N35">
+        <f>POISSON(N$27,$L34,FALSE)</f>
+        <v>0.36768654871205836</v>
+      </c>
+      <c r="O35">
+        <f>POISSON(O$27,$L34,FALSE)</f>
+        <v>0.1779531652005755</v>
+      </c>
+      <c r="P35">
+        <f>POISSON(P$27,$L34,FALSE)</f>
+        <v>5.7417255931405758E-2</v>
+      </c>
+      <c r="Q35">
+        <f>POISSON(Q$27,$L34,FALSE)</f>
+        <v>1.3894419670661838E-2</v>
+      </c>
+      <c r="R35">
+        <f>POISSON(R$27,$L34,FALSE)</f>
+        <v>2.6898519596981105E-3</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="V35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36" t="s">
         <v>176</v>
       </c>
-      <c r="B32">
+      <c r="B36">
         <v>97</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <v>67</v>
       </c>
-      <c r="D32">
+      <c r="D36">
         <v>60</v>
       </c>
-      <c r="E32">
+      <c r="E36">
         <v>10</v>
       </c>
-      <c r="F32">
+      <c r="F36">
         <v>9</v>
       </c>
-      <c r="G32">
+      <c r="G36">
         <v>6</v>
       </c>
-      <c r="H32">
+      <c r="H36">
         <v>4</v>
       </c>
-      <c r="I32">
+      <c r="I36">
         <v>12</v>
       </c>
-      <c r="J32">
+      <c r="J36">
         <v>6</v>
       </c>
-      <c r="K32">
+      <c r="K36">
         <f t="shared" si="0"/>
         <v>2.8851873884592503</v>
       </c>
-      <c r="L32">
+      <c r="L36">
         <f t="shared" si="1"/>
         <v>0.59785841760856628</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" t="s">
+      <c r="M36">
+        <f>POISSON(M$27,$K36,FALSE)</f>
+        <v>5.5844323974125691E-2</v>
+      </c>
+      <c r="N36">
+        <f>POISSON(N$27,$K36,FALSE)</f>
+        <v>0.16112133924718</v>
+      </c>
+      <c r="O36">
+        <f>POISSON(O$27,$K36,FALSE)</f>
+        <v>0.23243262800381409</v>
+      </c>
+      <c r="P36">
+        <f>POISSON(P$27,$K36,FALSE)</f>
+        <v>0.22353722899434825</v>
+      </c>
+      <c r="Q36">
+        <f>POISSON(Q$27,$K36,FALSE)</f>
+        <v>0.16123669848640526</v>
+      </c>
+      <c r="R36">
+        <f>POISSON(R$27,$K36,FALSE)</f>
+        <v>9.303961780595664E-2</v>
+      </c>
+      <c r="S36">
+        <v>2</v>
+      </c>
+      <c r="T36">
+        <v>2</v>
+      </c>
+      <c r="V36" t="s">
+        <v>187</v>
+      </c>
+      <c r="W36" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="M37">
+        <f>POISSON(M$27,$L36,FALSE)</f>
+        <v>0.54998822085701893</v>
+      </c>
+      <c r="N37">
+        <f>POISSON(N$27,$L36,FALSE)</f>
+        <v>0.32881508742492799</v>
+      </c>
+      <c r="O37">
+        <f>POISSON(O$27,$L36,FALSE)</f>
+        <v>9.8292433926844919E-2</v>
+      </c>
+      <c r="P37">
+        <f>POISSON(P$27,$L36,FALSE)</f>
+        <v>1.9588319670132685E-2</v>
+      </c>
+      <c r="Q37">
+        <f>POISSON(Q$27,$L36,FALSE)</f>
+        <v>2.9277604503990702E-3</v>
+      </c>
+      <c r="R37">
+        <f>POISSON(R$27,$L36,FALSE)</f>
+        <v>3.5007724600250625E-4</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="V37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38" t="s">
         <v>177</v>
       </c>
-      <c r="B33">
+      <c r="B38">
         <v>97</v>
       </c>
-      <c r="C33">
+      <c r="C38">
         <v>67</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <v>60</v>
       </c>
-      <c r="K33" t="e">
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>11</v>
+      </c>
+      <c r="I38">
+        <v>6</v>
+      </c>
+      <c r="J38">
+        <v>6</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L33" t="e">
+        <v>1.3848899464604401</v>
+      </c>
+      <c r="L38">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" t="s">
+        <v>2.1921475312314098</v>
+      </c>
+      <c r="M38">
+        <f>POISSON(M$27,$K38,FALSE)</f>
+        <v>0.25035135032789219</v>
+      </c>
+      <c r="N38">
+        <f>POISSON(N$27,$K38,FALSE)</f>
+        <v>0.34670906815189345</v>
+      </c>
+      <c r="O38">
+        <f>POISSON(O$27,$K38,FALSE)</f>
+        <v>0.2400769514151124</v>
+      </c>
+      <c r="P38">
+        <f>POISSON(P$27,$K38,FALSE)</f>
+        <v>0.11082671879722023</v>
+      </c>
+      <c r="Q38">
+        <f>POISSON(Q$27,$K38,FALSE)</f>
+        <v>3.8370702165367143E-2</v>
+      </c>
+      <c r="R38">
+        <f>POISSON(R$27,$K38,FALSE)</f>
+        <v>1.0627839933488958E-2</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="W38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="M39">
+        <f>POISSON(M$27,$L38,FALSE)</f>
+        <v>0.11167666179360297</v>
+      </c>
+      <c r="N39">
+        <f>POISSON(N$27,$L38,FALSE)</f>
+        <v>0.24481171844701186</v>
+      </c>
+      <c r="O39">
+        <f>POISSON(O$27,$L38,FALSE)</f>
+        <v>0.26833170210506802</v>
+      </c>
+      <c r="P39">
+        <f>POISSON(P$27,$L38,FALSE)</f>
+        <v>0.19607422610691563</v>
+      </c>
+      <c r="Q39">
+        <f>POISSON(Q$27,$L38,FALSE)</f>
+        <v>0.10745590767459608</v>
+      </c>
+      <c r="R39">
+        <f>POISSON(R$27,$L38,FALSE)</f>
+        <v>4.7111840545019226E-2</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
+      <c r="A40" t="s">
         <v>178</v>
       </c>
-      <c r="B34">
+      <c r="B40">
         <v>97</v>
       </c>
-      <c r="C34">
+      <c r="C40">
         <v>67</v>
       </c>
-      <c r="D34">
+      <c r="D40">
         <v>60</v>
       </c>
-      <c r="K34" t="e">
+      <c r="E40">
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>6</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L34" t="e">
+        <v>3.2458358120166571</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" t="s">
+        <v>0.19928613920285543</v>
+      </c>
+      <c r="M40">
+        <f>POISSON(M$27,$K40,FALSE)</f>
+        <v>3.8936007570496367E-2</v>
+      </c>
+      <c r="N40">
+        <f>POISSON(N$27,$K40,FALSE)</f>
+        <v>0.12637988774926875</v>
+      </c>
+      <c r="O40">
+        <f>POISSON(O$27,$K40,FALSE)</f>
+        <v>0.20510418278761086</v>
+      </c>
+      <c r="P40">
+        <f>POISSON(P$27,$K40,FALSE)</f>
+        <v>0.22191150056214592</v>
+      </c>
+      <c r="Q40">
+        <f>POISSON(Q$27,$K40,FALSE)</f>
+        <v>0.18007207390574195</v>
+      </c>
+      <c r="R40">
+        <f>POISSON(R$27,$K40,FALSE)</f>
+        <v>0.11689687724547347</v>
+      </c>
+      <c r="S40">
+        <v>3</v>
+      </c>
+      <c r="T40">
+        <v>3</v>
+      </c>
+      <c r="V40" t="s">
+        <v>187</v>
+      </c>
+      <c r="W40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
+      <c r="M41">
+        <f>POISSON(M$27,$L40,FALSE)</f>
+        <v>0.81931542152713499</v>
+      </c>
+      <c r="N41">
+        <f>POISSON(N$27,$L40,FALSE)</f>
+        <v>0.16327820714550281</v>
+      </c>
+      <c r="O41">
+        <f>POISSON(O$27,$L40,FALSE)</f>
+        <v>1.6269541758995667E-2</v>
+      </c>
+      <c r="P41">
+        <f>POISSON(P$27,$L40,FALSE)</f>
+        <v>1.08076472124996E-3</v>
+      </c>
+      <c r="Q41">
+        <f>POISSON(Q$27,$L40,FALSE)</f>
+        <v>5.3845357171138704E-5</v>
+      </c>
+      <c r="R41">
+        <f>POISSON(R$27,$L40,FALSE)</f>
+        <v>2.1461266689270033E-6</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>2</v>
+      </c>
+      <c r="V41" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="A42" t="s">
         <v>179</v>
       </c>
-      <c r="B35">
+      <c r="B42">
         <v>97</v>
       </c>
-      <c r="C35">
+      <c r="C42">
         <v>67</v>
       </c>
-      <c r="D35">
+      <c r="D42">
         <v>60</v>
       </c>
-      <c r="K35" t="e">
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>9</v>
+      </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+      <c r="J42">
+        <v>6</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L35" t="e">
+        <v>1.3464207812809834</v>
+      </c>
+      <c r="L42">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" t="s">
+        <v>0.74732302201070799</v>
+      </c>
+      <c r="M42">
+        <f>POISSON(M$27,$K42,FALSE)</f>
+        <v>0.26016980076086382</v>
+      </c>
+      <c r="N42">
+        <f>POISSON(N$27,$K42,FALSE)</f>
+        <v>0.35029802640616009</v>
+      </c>
+      <c r="O42">
+        <f>POISSON(O$27,$K42,FALSE)</f>
+        <v>0.23582427119748431</v>
+      </c>
+      <c r="P42">
+        <f>POISSON(P$27,$K42,FALSE)</f>
+        <v>0.10583956649024512</v>
+      </c>
+      <c r="Q42">
+        <f>POISSON(Q$27,$K42,FALSE)</f>
+        <v>3.5626147951059103E-2</v>
+      </c>
+      <c r="R42">
+        <f>POISSON(R$27,$K42,FALSE)</f>
+        <v>9.5935571916593819E-3</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>2</v>
+      </c>
+      <c r="V42" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
+      <c r="M43">
+        <f>POISSON(M$27,$L42,FALSE)</f>
+        <v>0.47363276165612017</v>
+      </c>
+      <c r="N43">
+        <f>POISSON(N$27,$L42,FALSE)</f>
+        <v>0.35395666676412912</v>
+      </c>
+      <c r="O43">
+        <f>POISSON(O$27,$L42,FALSE)</f>
+        <v>0.13225998293350305</v>
+      </c>
+      <c r="P43">
+        <f>POISSON(P$27,$L42,FALSE)</f>
+        <v>3.2946976712316722E-2</v>
+      </c>
+      <c r="Q43">
+        <f>POISSON(Q$27,$L42,FALSE)</f>
+        <v>6.1555085506912388E-3</v>
+      </c>
+      <c r="R43">
+        <f>POISSON(R$27,$L42,FALSE)</f>
+        <v>9.2003065042306606E-4</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="V43" t="s">
+        <v>187</v>
+      </c>
+      <c r="W43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
+      <c r="A44" t="s">
         <v>180</v>
       </c>
-      <c r="B36">
+      <c r="B44">
         <v>97</v>
       </c>
-      <c r="C36">
+      <c r="C44">
         <v>67</v>
       </c>
-      <c r="D36">
+      <c r="D44">
         <v>60</v>
       </c>
-      <c r="K36" t="e">
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>6</v>
+      </c>
+      <c r="H44">
+        <v>12</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>6</v>
+      </c>
+      <c r="K44">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L36" t="e">
+        <v>0.43277810826888752</v>
+      </c>
+      <c r="L44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.5942891136228434</v>
+      </c>
+      <c r="M44">
+        <f>POISSON(M$27,$K44,FALSE)</f>
+        <v>0.64870441798265899</v>
+      </c>
+      <c r="N44">
+        <f>POISSON(N$27,$K44,FALSE)</f>
+        <v>0.28074507084020489</v>
+      </c>
+      <c r="O44">
+        <f>POISSON(O$27,$K44,FALSE)</f>
+        <v>6.0750160332019333E-2</v>
+      </c>
+      <c r="P44">
+        <f>POISSON(P$27,$K44,FALSE)</f>
+        <v>8.76377982184098E-3</v>
+      </c>
+      <c r="Q44">
+        <f>POISSON(Q$27,$K44,FALSE)</f>
+        <v>9.4819301314534685E-4</v>
+      </c>
+      <c r="R44">
+        <f>POISSON(R$27,$K44,FALSE)</f>
+        <v>8.2071435700563919E-5</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44" t="s">
+        <v>187</v>
+      </c>
+      <c r="V44" t="s">
+        <v>187</v>
+      </c>
+      <c r="W44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="M45">
+        <f>POISSON(M$27,$L44,FALSE)</f>
+        <v>0.2030528246942897</v>
+      </c>
+      <c r="N45">
+        <f>POISSON(N$27,$L44,FALSE)</f>
+        <v>0.32372490790047376</v>
+      </c>
+      <c r="O45">
+        <f>POISSON(O$27,$L44,FALSE)</f>
+        <v>0.2580555482371415</v>
+      </c>
+      <c r="P45">
+        <f>POISSON(P$27,$L44,FALSE)</f>
+        <v>0.13713838375481641</v>
+      </c>
+      <c r="Q45">
+        <f>POISSON(Q$27,$L44,FALSE)</f>
+        <v>5.4659558070033906E-2</v>
+      </c>
+      <c r="R45">
+        <f>POISSON(R$27,$L44,FALSE)</f>
+        <v>1.7428627677298136E-2</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45" t="s">
+        <v>187</v>
+      </c>
+      <c r="V45" t="s">
+        <v>187</v>
+      </c>
+      <c r="W45" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
+      <c r="U46">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="V46">
+        <f>6/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="W46" s="10">
+        <f>6/20</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="O47">
+        <f>SUM(O29:P29)</f>
+        <v>0.23801637974010353</v>
+      </c>
+      <c r="Q47">
+        <f>SUM(Q29:R29)</f>
+        <v>1.7055680731226146E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added handling for yellow card and red card points deductions.
</commit_message>
<xml_diff>
--- a/data/poission.xlsx
+++ b/data/poission.xlsx
@@ -15,13 +15,14 @@
     <sheet name="Average Goals Calc" sheetId="2" r:id="rId6"/>
     <sheet name="Six Games" sheetId="3" r:id="rId7"/>
     <sheet name="Mignolet Points" sheetId="5" r:id="rId8"/>
+    <sheet name="GoalsRatioPerGame" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="199">
   <si>
     <t>Wigan</t>
   </si>
@@ -597,6 +598,27 @@
   </si>
   <si>
     <t>Kone</t>
+  </si>
+  <si>
+    <t>with points per game</t>
+  </si>
+  <si>
+    <t>maloney goals</t>
+  </si>
+  <si>
+    <t>maloney games</t>
+  </si>
+  <si>
+    <t>goals ratio</t>
+  </si>
+  <si>
+    <t>goals per game ratio</t>
+  </si>
+  <si>
+    <t>other player goals</t>
+  </si>
+  <si>
+    <t>other player games</t>
   </si>
 </sst>
 </file>
@@ -967,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3479,6 +3501,9 @@
       <c r="Y38" s="5"/>
     </row>
     <row r="39" spans="1:30">
+      <c r="D39" t="s">
+        <v>192</v>
+      </c>
       <c r="K39">
         <f>2.88*0.2*3</f>
         <v>1.7279999999999998</v>
@@ -3522,6 +3547,21 @@
       <c r="A40" t="s">
         <v>191</v>
       </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="D40">
+        <f>((90*4)+24)/90</f>
+        <v>4.2666666666666666</v>
+      </c>
+      <c r="E40">
+        <f>3/D40</f>
+        <v>0.703125</v>
+      </c>
       <c r="K40">
         <f>SUM(K36:K39)</f>
         <v>4.9546069621303506</v>
@@ -3548,6 +3588,17 @@
       <c r="Y40" s="6"/>
     </row>
     <row r="41" spans="1:30">
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41">
+        <f>3/5*(4)*2.88</f>
+        <v>6.9119999999999999</v>
+      </c>
+      <c r="E41">
+        <f>((3/(4/5))/5)*4*2.88</f>
+        <v>8.64</v>
+      </c>
       <c r="R41" s="6">
         <v>1.7894162805133858E-3</v>
       </c>
@@ -3581,6 +3632,17 @@
       </c>
     </row>
     <row r="42" spans="1:30">
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42">
+        <f>1/5*(3)*2.88</f>
+        <v>1.7280000000000002</v>
+      </c>
+      <c r="E42">
+        <f>(1/(4/5))/5*(3)*2.88</f>
+        <v>2.16</v>
+      </c>
       <c r="R42">
         <f>SUM(R36:R41)</f>
         <v>5.5357490301792232E-2</v>
@@ -3607,6 +3669,14 @@
       </c>
     </row>
     <row r="43" spans="1:30">
+      <c r="C43">
+        <f>SUM(C40:C42)</f>
+        <v>9.24</v>
+      </c>
+      <c r="E43">
+        <f>SUM(E40:E42)</f>
+        <v>11.503125000000001</v>
+      </c>
       <c r="R43">
         <f>R42*4</f>
         <v>0.22142996120716893</v>
@@ -16045,4 +16115,223 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f>C2/(A2+C2)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <f>(C2/(A2+C2))*B2/D2</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>C3/(A3+C3)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F3">
+        <f>(C3/(A3+C3))*B3/D3</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <f>C4/(A4+C4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <f>(C4/(A4+C4))*B4/D4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>C5/(A5+C5)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F5">
+        <f>(C5/(A5+C5))*B5/D5</f>
+        <v>0.41666666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f>C6/(A6+C6)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <f>((B6/D6)*C6)/(A6+((B6/D6)*C6))</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f>C7/(A7+C7)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <f>((B7/D7)*C7)/(A7+((B7/D7)*C7))</f>
+        <v>0.23809523809523808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <f>C8/(A8+C8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <f>((B8/D8)*C8)/(A8+((B8/D8)*C8))</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>C9/(A9+C9)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F9">
+        <f>((B9/D9)*C9)/(A9+((B9/D9)*C9))</f>
+        <v>0.38461538461538464</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>